<commit_message>
add: log of IC50 and selection of relevant peptides
</commit_message>
<xml_diff>
--- a/resources/AMPs_DB_IC50.xlsx
+++ b/resources/AMPs_DB_IC50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33652\Desktop\Anti-microbial peptides\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mag\filrouge\Anti-Fungi-Peptide\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2794DB5B-FFA3-43A8-9D54-5208F94551A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9587D91-B65A-48E3-9966-E075F16117E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{A24027CC-C66B-4241-9FFD-46A096C7D170}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A24027CC-C66B-4241-9FFD-46A096C7D170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
   <si>
     <t>RWRWKRWWW</t>
   </si>
@@ -641,25 +641,31 @@
     <t>GSRRFGWNR</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>Cumulative Vote</t>
-  </si>
-  <si>
-    <t>Rel IC50</t>
-  </si>
-  <si>
     <t>charge</t>
   </si>
   <si>
-    <t xml:space="preserve">hydrophobic fraction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrophobic moment </t>
+    <t>select</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>cumulative_vote</t>
+  </si>
+  <si>
+    <t>rel_IC50</t>
+  </si>
+  <si>
+    <t>hydrophobic_fraction</t>
+  </si>
+  <si>
+    <t>hydrophobic_moment</t>
+  </si>
+  <si>
+    <t>log_IC50</t>
   </si>
 </sst>
 </file>
@@ -701,7 +707,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -715,26 +728,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BCF5A7A-FBC5-40BE-96C1-CE4D86689159}" name="Table1" displayName="Table1" ref="A1:G201" totalsRowShown="0">
-  <autoFilter ref="A1:G201" xr:uid="{2BCF5A7A-FBC5-40BE-96C1-CE4D86689159}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BCF5A7A-FBC5-40BE-96C1-CE4D86689159}" name="Table1" displayName="Table1" ref="A1:I201" totalsRowShown="0">
+  <autoFilter ref="A1:I201" xr:uid="{2BCF5A7A-FBC5-40BE-96C1-CE4D86689159}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G201">
     <sortCondition ref="D1:D201"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EC0D64DC-BA52-4F66-B41C-424E3979A16A}" name="Rank"/>
-    <tableColumn id="2" xr3:uid="{82EE582C-2484-4FE0-B96E-89CF37B25286}" name="Sequence"/>
-    <tableColumn id="3" xr3:uid="{A7C4D70E-CA6C-4EAD-9766-3AFB5575F5BC}" name="Cumulative Vote"/>
-    <tableColumn id="4" xr3:uid="{D1B735F4-2F15-4CD6-9BFD-BCAC1B5000CA}" name="Rel IC50"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{EC0D64DC-BA52-4F66-B41C-424E3979A16A}" name="rank"/>
+    <tableColumn id="2" xr3:uid="{82EE582C-2484-4FE0-B96E-89CF37B25286}" name="sequence"/>
+    <tableColumn id="3" xr3:uid="{A7C4D70E-CA6C-4EAD-9766-3AFB5575F5BC}" name="cumulative_vote"/>
+    <tableColumn id="4" xr3:uid="{D1B735F4-2F15-4CD6-9BFD-BCAC1B5000CA}" name="rel_IC50"/>
     <tableColumn id="5" xr3:uid="{663F4900-F16D-48F4-AB2C-F966C17CB563}" name="charge"/>
-    <tableColumn id="6" xr3:uid="{33D301DD-DC6E-48CE-83D8-A9B2DA4C4167}" name="hydrophobic fraction "/>
-    <tableColumn id="7" xr3:uid="{D5596435-A891-496E-BA3F-3C98773BE135}" name="hydrophobic moment "/>
+    <tableColumn id="6" xr3:uid="{33D301DD-DC6E-48CE-83D8-A9B2DA4C4167}" name="hydrophobic_fraction"/>
+    <tableColumn id="7" xr3:uid="{D5596435-A891-496E-BA3F-3C98773BE135}" name="hydrophobic_moment"/>
+    <tableColumn id="8" xr3:uid="{5BFA329E-F11E-4112-A1DC-D6965C80387B}" name="select" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{2F7CC899-021E-4FCE-88BB-E7756E38082F}" name="log_IC50" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1030,47 +1045,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B34B5B7-C77F-41B2-9E61-683CE7882437}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="6.9296875" customWidth="1"/>
-    <col min="6" max="6" width="6.46484375" customWidth="1"/>
-    <col min="7" max="7" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
         <v>200</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
         <v>201</v>
       </c>
-      <c r="C1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="I1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1092,8 +1113,14 @@
       <c r="G2">
         <v>4.6500000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>-1.3979400086720375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1115,8 +1142,14 @@
       <c r="G3">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>-1.0969100130080565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -1138,8 +1171,14 @@
       <c r="G4">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>-0.92081875395237522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>24897</v>
       </c>
@@ -1161,8 +1200,14 @@
       <c r="G5">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>-0.92081875395237522</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1184,8 +1229,14 @@
       <c r="G6">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>-0.88605664769316317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>36</v>
       </c>
@@ -1207,8 +1258,14 @@
       <c r="G7">
         <v>5.89</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>-0.88605664769316317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -1230,8 +1287,14 @@
       <c r="G8">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>-0.85387196432176193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>19</v>
       </c>
@@ -1253,8 +1316,14 @@
       <c r="G9">
         <v>4.29</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>-0.82390874094431876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>37</v>
       </c>
@@ -1276,8 +1345,14 @@
       <c r="G10">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>-0.82390874094431876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>24919</v>
       </c>
@@ -1299,8 +1374,14 @@
       <c r="G11">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>-0.82390874094431876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>24915</v>
       </c>
@@ -1322,8 +1403,14 @@
       <c r="G12">
         <v>3.53</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>-0.79588001734407521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>33</v>
       </c>
@@ -1345,8 +1432,14 @@
       <c r="G13">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>-0.74472749489669399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>24900</v>
       </c>
@@ -1368,8 +1461,14 @@
       <c r="G14">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>-0.74472749489669399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>24910</v>
       </c>
@@ -1391,8 +1490,14 @@
       <c r="G15">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>-0.74472749489669399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>44</v>
       </c>
@@ -1414,8 +1519,14 @@
       <c r="G16">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>-0.72124639904717103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>48</v>
       </c>
@@ -1437,8 +1548,14 @@
       <c r="G17">
         <v>2.41</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>-0.72124639904717103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1460,8 +1577,14 @@
       <c r="G18">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>-0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>25</v>
       </c>
@@ -1483,8 +1606,14 @@
       <c r="G19">
         <v>3.32</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>-0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>30</v>
       </c>
@@ -1506,8 +1635,14 @@
       <c r="G20">
         <v>5.14</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>-0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>45</v>
       </c>
@@ -1529,8 +1664,14 @@
       <c r="G21">
         <v>4.66</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>-0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -1552,8 +1693,14 @@
       <c r="G22">
         <v>6.32</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>-0.6777807052660807</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>31</v>
       </c>
@@ -1575,8 +1722,14 @@
       <c r="G23">
         <v>5.09</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>-0.6777807052660807</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>32</v>
       </c>
@@ -1598,8 +1751,14 @@
       <c r="G24">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>-0.6777807052660807</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>35</v>
       </c>
@@ -1621,8 +1780,14 @@
       <c r="G25">
         <v>5.05</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>-0.6777807052660807</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>39</v>
       </c>
@@ -1644,8 +1809,14 @@
       <c r="G26">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>-0.6777807052660807</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>11</v>
       </c>
@@ -1667,8 +1838,14 @@
       <c r="G27">
         <v>4.1900000000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>-0.65757731917779372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>17</v>
       </c>
@@ -1690,8 +1867,14 @@
       <c r="G28">
         <v>2.98</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>-0.65757731917779372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>49</v>
       </c>
@@ -1713,8 +1896,14 @@
       <c r="G29">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>-0.65757731917779372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>24913</v>
       </c>
@@ -1736,8 +1925,14 @@
       <c r="G30">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>-0.65757731917779372</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>13</v>
       </c>
@@ -1759,8 +1954,14 @@
       <c r="G31">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>47</v>
       </c>
@@ -1782,8 +1983,14 @@
       <c r="G32">
         <v>4.9400000000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>50</v>
       </c>
@@ -1805,8 +2012,14 @@
       <c r="G33">
         <v>5.39</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>24926</v>
       </c>
@@ -1828,8 +2041,14 @@
       <c r="G34">
         <v>3.68</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>24933</v>
       </c>
@@ -1851,8 +2070,14 @@
       <c r="G35">
         <v>2.56</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24937</v>
       </c>
@@ -1874,8 +2099,14 @@
       <c r="G36">
         <v>2.5499999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>-0.63827216398240705</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16</v>
       </c>
@@ -1897,8 +2128,14 @@
       <c r="G37">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>-0.61978875828839397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>24</v>
       </c>
@@ -1920,8 +2157,14 @@
       <c r="G38">
         <v>5.23</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>-0.61978875828839397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>29</v>
       </c>
@@ -1943,8 +2186,14 @@
       <c r="G39">
         <v>4.1100000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>-0.61978875828839397</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>24923</v>
       </c>
@@ -1966,8 +2215,14 @@
       <c r="G40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>-0.61978875828839397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>24944</v>
       </c>
@@ -1989,8 +2244,14 @@
       <c r="G41">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>-0.61978875828839397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2012,8 +2273,14 @@
       <c r="G42">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>-0.6020599913279624</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>22</v>
       </c>
@@ -2035,8 +2302,14 @@
       <c r="G43">
         <v>2.96</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>-0.6020599913279624</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>26</v>
       </c>
@@ -2058,8 +2331,14 @@
       <c r="G44">
         <v>2.2799999999999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>-0.6020599913279624</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2081,8 +2360,14 @@
       <c r="G45">
         <v>5.94</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>-0.58502665202918203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>24908</v>
       </c>
@@ -2104,8 +2389,14 @@
       <c r="G46">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>-0.58502665202918203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>24914</v>
       </c>
@@ -2127,8 +2418,14 @@
       <c r="G47">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>-0.58502665202918203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>24922</v>
       </c>
@@ -2150,8 +2447,14 @@
       <c r="G48">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>-0.58502665202918203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>24931</v>
       </c>
@@ -2173,8 +2476,14 @@
       <c r="G49">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>-0.58502665202918203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>14</v>
       </c>
@@ -2196,8 +2505,14 @@
       <c r="G50">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>-0.56863623584101264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>24898</v>
       </c>
@@ -2219,8 +2534,14 @@
       <c r="G51">
         <v>2.27</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>-0.56863623584101264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2242,8 +2563,14 @@
       <c r="G52">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>-0.55284196865778079</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>21</v>
       </c>
@@ -2265,8 +2592,14 @@
       <c r="G53">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>-0.55284196865778079</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>27</v>
       </c>
@@ -2288,8 +2621,14 @@
       <c r="G54">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>-0.55284196865778079</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>40</v>
       </c>
@@ -2311,8 +2650,14 @@
       <c r="G55">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>-0.55284196865778079</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>46</v>
       </c>
@@ -2334,8 +2679,14 @@
       <c r="G56">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>-0.55284196865778079</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>24921</v>
       </c>
@@ -2357,8 +2708,14 @@
       <c r="G57">
         <v>3.52</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>-0.53760200210104392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>28</v>
       </c>
@@ -2380,8 +2737,14 @@
       <c r="G58">
         <v>2.57</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>-0.52287874528033762</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>24928</v>
       </c>
@@ -2403,8 +2766,14 @@
       <c r="G59">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>-0.52287874528033762</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>15</v>
       </c>
@@ -2426,8 +2795,14 @@
       <c r="G60">
         <v>5.44</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>-0.50863830616572736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>23</v>
       </c>
@@ -2449,8 +2824,14 @@
       <c r="G61">
         <v>2.09</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>-0.50863830616572736</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>24936</v>
       </c>
@@ -2472,8 +2853,14 @@
       <c r="G62">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>-0.50863830616572736</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>24941</v>
       </c>
@@ -2495,8 +2882,14 @@
       <c r="G63">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>-0.49485002168009401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>74635</v>
       </c>
@@ -2518,8 +2911,14 @@
       <c r="G64">
         <v>3.76</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>-0.49485002168009401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>24901</v>
       </c>
@@ -2541,8 +2940,14 @@
       <c r="G65">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>-0.48148606012211248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>24916</v>
       </c>
@@ -2564,8 +2969,14 @@
       <c r="G66">
         <v>3.74</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>-0.48148606012211248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>24943</v>
       </c>
@@ -2587,8 +2998,14 @@
       <c r="G67">
         <v>3.07</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>-0.48148606012211248</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>24899</v>
       </c>
@@ -2610,8 +3027,14 @@
       <c r="G68">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>-0.46852108295774486</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>42</v>
       </c>
@@ -2633,8 +3056,14 @@
       <c r="G69">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>-0.45593195564972439</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>24904</v>
       </c>
@@ -2656,8 +3085,14 @@
       <c r="G70">
         <v>2.92</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>-0.45593195564972439</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>18</v>
       </c>
@@ -2679,8 +3114,14 @@
       <c r="G71">
         <v>4.1900000000000004</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>-0.44369749923271273</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>24896</v>
       </c>
@@ -2702,8 +3143,14 @@
       <c r="G72">
         <v>4.0599999999999996</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>-0.44369749923271273</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>24942</v>
       </c>
@@ -2725,8 +3172,14 @@
       <c r="G73">
         <v>5.24</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>-0.42021640338318983</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
@@ -2748,8 +3201,14 @@
       <c r="G74">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>-0.40893539297350079</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>24938</v>
       </c>
@@ -2771,8 +3230,14 @@
       <c r="G75">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>-0.40893539297350079</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
@@ -2794,8 +3259,14 @@
       <c r="G76">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>-0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>24920</v>
       </c>
@@ -2817,8 +3288,14 @@
       <c r="G77">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>-0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>24906</v>
       </c>
@@ -2840,8 +3317,14 @@
       <c r="G78">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>-0.38721614328026455</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>6</v>
       </c>
@@ -2863,8 +3346,14 @@
       <c r="G79">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>-0.36653154442041347</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>74640</v>
       </c>
@@ -2886,8 +3375,14 @@
       <c r="G80">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>-0.35654732351381258</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>24927</v>
       </c>
@@ -2909,8 +3404,14 @@
       <c r="G81">
         <v>2.99</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>-0.33724216831842591</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>24929</v>
       </c>
@@ -2932,8 +3433,14 @@
       <c r="G82">
         <v>2.68</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>-0.33724216831842591</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>24940</v>
       </c>
@@ -2955,8 +3462,14 @@
       <c r="G83">
         <v>4.8899999999999997</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>-0.3010299956639812</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>24909</v>
       </c>
@@ -2978,8 +3491,14 @@
       <c r="G84">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>-0.29242982390206362</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>24932</v>
       </c>
@@ -3001,8 +3520,14 @@
       <c r="G85">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>-0.28399665636520083</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>24918</v>
       </c>
@@ -3024,8 +3549,14 @@
       <c r="G86">
         <v>1.58</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>-0.27572413039921095</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>24905</v>
       </c>
@@ -3047,8 +3578,14 @@
       <c r="G87">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>-0.26760624017703144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>24935</v>
       </c>
@@ -3070,8 +3607,14 @@
       <c r="G88">
         <v>2.62</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>-0.26760624017703144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>24917</v>
       </c>
@@ -3093,8 +3636,14 @@
       <c r="G89">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>-0.24412514432750865</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>41</v>
       </c>
@@ -3116,8 +3665,14 @@
       <c r="G90">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>-0.22914798835785583</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>24895</v>
       </c>
@@ -3139,8 +3694,14 @@
       <c r="G91">
         <v>4.24</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>-0.21467016498923297</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>38</v>
       </c>
@@ -3162,8 +3723,14 @@
       <c r="G92">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>-0.16749108729376366</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>24925</v>
       </c>
@@ -3185,8 +3752,14 @@
       <c r="G93">
         <v>2.59</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>-0.15490195998574319</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>74639</v>
       </c>
@@ -3208,8 +3781,14 @@
       <c r="G94">
         <v>2.63</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>-0.14266750356873156</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>24902</v>
       </c>
@@ -3231,8 +3810,14 @@
       <c r="G95">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>-0.11918640771920865</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>24912</v>
       </c>
@@ -3254,8 +3839,14 @@
       <c r="G96">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>-7.0581074285707285E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>24930</v>
       </c>
@@ -3277,8 +3868,14 @@
       <c r="G97">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>-5.551732784983137E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>24907</v>
       </c>
@@ -3300,8 +3897,14 @@
       <c r="G98">
         <v>4.67</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>-2.2276394711152253E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>24911</v>
       </c>
@@ -3323,8 +3926,14 @@
       <c r="G99">
         <v>3.44</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>-4.3648054024500883E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>74648</v>
       </c>
@@ -3346,8 +3955,14 @@
       <c r="G100">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>2.5305865264770262E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>74644</v>
       </c>
@@ -3369,8 +3984,14 @@
       <c r="G101">
         <v>2.84</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>6.445798922691845E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>74681</v>
       </c>
@@ -3392,8 +4013,14 @@
       <c r="G102">
         <v>5.39</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>8.2785370316450071E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>24924</v>
       </c>
@@ -3415,8 +4042,14 @@
       <c r="G103">
         <v>3.11</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>8.9905111439397931E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>74677</v>
       </c>
@@ -3438,8 +4071,14 @@
       <c r="G104">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>0.17897694729316943</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>74664</v>
       </c>
@@ -3461,8 +4100,14 @@
       <c r="G105">
         <v>1.33</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>0.2576785748691845</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>34</v>
       </c>
@@ -3484,8 +4129,14 @@
       <c r="G106">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>0.26007138798507479</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>24939</v>
       </c>
@@ -3507,8 +4158,14 @@
       <c r="G107">
         <v>2.84</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>0.26007138798507479</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>74670</v>
       </c>
@@ -3530,8 +4187,14 @@
       <c r="G108">
         <v>4.59</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>0.33243845991560533</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>74636</v>
       </c>
@@ -3553,8 +4216,14 @@
       <c r="G109">
         <v>3.69</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>0.34635297445063867</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>74651</v>
       </c>
@@ -3576,8 +4245,14 @@
       <c r="G110">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>0.35024801833416286</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>99556</v>
       </c>
@@ -3599,8 +4274,14 @@
       <c r="G111">
         <v>2.29</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111">
+        <v>0.36172783601759284</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>74669</v>
       </c>
@@ -3622,8 +4303,14 @@
       <c r="G112">
         <v>2.63</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>74645</v>
       </c>
@@ -3645,8 +4332,14 @@
       <c r="G113">
         <v>5.36</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0.41830129131974547</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>74653</v>
       </c>
@@ -3668,8 +4361,14 @@
       <c r="G114">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0.43775056282038799</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>74643</v>
       </c>
@@ -3691,8 +4390,14 @@
       <c r="G115">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0.44247976906444858</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>74659</v>
       </c>
@@ -3714,8 +4419,14 @@
       <c r="G116">
         <v>3.94</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>0.44560420327359757</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>74637</v>
       </c>
@@ -3737,8 +4448,14 @@
       <c r="G117">
         <v>3.91</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117">
+        <v>0.4668676203541095</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>24903</v>
       </c>
@@ -3760,8 +4477,14 @@
       <c r="G118">
         <v>4.1100000000000003</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>0.48287358360875376</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>74642</v>
       </c>
@@ -3783,8 +4506,14 @@
       <c r="G119">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0.50920252233110286</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>74652</v>
       </c>
@@ -3806,8 +4535,14 @@
       <c r="G120">
         <v>3.41</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>0.53019969820308221</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>74650</v>
       </c>
@@ -3829,8 +4564,14 @@
       <c r="G121">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0.54406804435027567</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>74646</v>
       </c>
@@ -3852,8 +4593,14 @@
       <c r="G122">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0.55509444857831913</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>74678</v>
       </c>
@@ -3875,8 +4622,14 @@
       <c r="G123">
         <v>4.9400000000000004</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>0.58319877396862274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>74634</v>
       </c>
@@ -3898,8 +4651,14 @@
       <c r="G124">
         <v>4.46</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0.62531245096167387</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>74633</v>
       </c>
@@ -3921,8 +4680,14 @@
       <c r="G125">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>0.62838893005031149</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>74667</v>
       </c>
@@ -3944,8 +4709,14 @@
       <c r="G126">
         <v>2.92</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>0.64147411050409953</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>74674</v>
       </c>
@@ -3967,8 +4738,14 @@
       <c r="G127">
         <v>5.94</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0.66464197555612547</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>74641</v>
       </c>
@@ -3990,8 +4767,14 @@
       <c r="G128">
         <v>2.91</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>0.68841982200271057</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>74662</v>
       </c>
@@ -4013,8 +4796,14 @@
       <c r="G129">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>0.69284691927722997</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>74671</v>
       </c>
@@ -4036,8 +4825,14 @@
       <c r="G130">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>0.70842090013471271</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>74647</v>
       </c>
@@ -4059,8 +4854,14 @@
       <c r="G131">
         <v>2.33</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>0.7307822756663892</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>74679</v>
       </c>
@@ -4082,8 +4883,14 @@
       <c r="G132">
         <v>2.41</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>0.7512791039833423</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>74638</v>
       </c>
@@ -4105,8 +4912,14 @@
       <c r="G133">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>0.75281643118827146</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>99557</v>
       </c>
@@ -4128,8 +4941,14 @@
       <c r="G134">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
+        <v>0.75663610824584804</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>99558</v>
       </c>
@@ -4151,8 +4970,14 @@
       <c r="G135">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135">
+        <v>0.78175537465246892</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>99540</v>
       </c>
@@ -4174,8 +4999,14 @@
       <c r="G136">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H136">
+        <v>0</v>
+      </c>
+      <c r="I136">
+        <v>0.79169064902011799</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>74668</v>
       </c>
@@ -4197,8 +5028,14 @@
       <c r="G137">
         <v>3.04</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
+        <v>0.79934054945358168</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>99552</v>
       </c>
@@ -4220,8 +5057,14 @@
       <c r="G138">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>0.80071707828238503</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>74666</v>
       </c>
@@ -4243,8 +5086,14 @@
       <c r="G139">
         <v>3.29</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>0.80753502806885324</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>99572</v>
       </c>
@@ -4266,8 +5115,14 @@
       <c r="G140">
         <v>2.88</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>0.80955971463526777</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>74665</v>
       </c>
@@ -4289,8 +5144,14 @@
       <c r="G141">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0.81291335664285558</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>74676</v>
       </c>
@@ -4312,8 +5173,14 @@
       <c r="G142">
         <v>4.66</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H142">
+        <v>0</v>
+      </c>
+      <c r="I142">
+        <v>0.81291335664285558</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>74656</v>
       </c>
@@ -4335,8 +5202,14 @@
       <c r="G143">
         <v>3.08</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0.81888541459400987</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>99551</v>
       </c>
@@ -4358,8 +5231,14 @@
       <c r="G144">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0.82282164530310464</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>74682</v>
       </c>
@@ -4381,8 +5260,14 @@
       <c r="G145">
         <v>4.24</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0.82347422917030111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>99562</v>
       </c>
@@ -4404,8 +5289,14 @@
       <c r="G146">
         <v>2.87</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H146">
+        <v>0</v>
+      </c>
+      <c r="I146">
+        <v>0.82930377283102497</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>74663</v>
       </c>
@@ -4427,8 +5318,14 @@
       <c r="G147">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H147">
+        <v>0</v>
+      </c>
+      <c r="I147">
+        <v>0.83186977428050168</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>99573</v>
       </c>
@@ -4450,8 +5347,14 @@
       <c r="G148">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>0.84073323461180671</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>99554</v>
       </c>
@@ -4473,8 +5376,14 @@
       <c r="G149">
         <v>3.81</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0.84880470105180372</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>99559</v>
       </c>
@@ -4496,8 +5405,14 @@
       <c r="G150">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>0.84941941379689945</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>74675</v>
       </c>
@@ -4519,8 +5434,14 @@
       <c r="G151">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>0.85003325768976901</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>99555</v>
       </c>
@@ -4542,8 +5463,14 @@
       <c r="G152">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H152">
+        <v>0</v>
+      </c>
+      <c r="I152">
+        <v>0.85973856619714695</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>99571</v>
       </c>
@@ -4565,8 +5492,14 @@
       <c r="G153">
         <v>1.1299999999999999</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>0.86805636182304158</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>99560</v>
       </c>
@@ -4588,8 +5521,14 @@
       <c r="G154">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0.88930170250631024</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>99550</v>
       </c>
@@ -4611,8 +5550,14 @@
       <c r="G155">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0.89817648349767654</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>99561</v>
       </c>
@@ -4634,8 +5579,14 @@
       <c r="G156">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0.89817648349767654</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>99543</v>
       </c>
@@ -4657,8 +5608,14 @@
       <c r="G157">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0.90036712865647028</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>99548</v>
       </c>
@@ -4680,8 +5637,14 @@
       <c r="G158">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0.90145832139611237</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>99574</v>
       </c>
@@ -4703,8 +5666,14 @@
       <c r="G159">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0.90525604874845123</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>99577</v>
       </c>
@@ -4726,8 +5695,14 @@
       <c r="G160">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0.90848501887864974</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>99533</v>
       </c>
@@ -4749,8 +5724,14 @@
       <c r="G161">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>0.91169015875386117</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>99567</v>
       </c>
@@ -4772,8 +5753,14 @@
       <c r="G162">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H162">
+        <v>0</v>
+      </c>
+      <c r="I162">
+        <v>0.9122220565324155</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>74655</v>
       </c>
@@ -4795,8 +5782,14 @@
       <c r="G163">
         <v>4.5199999999999996</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>0.91275330367132301</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>99536</v>
       </c>
@@ -4818,8 +5811,14 @@
       <c r="G164">
         <v>3.28</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <v>0.91381385238371671</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>74660</v>
       </c>
@@ -4841,8 +5840,14 @@
       <c r="G165">
         <v>3.54</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>0.91487181754005042</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>99549</v>
       </c>
@@ -4864,8 +5869,14 @@
       <c r="G166">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H166">
+        <v>0</v>
+      </c>
+      <c r="I166">
+        <v>0.91698004732038219</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>99569</v>
       </c>
@@ -4887,8 +5898,14 @@
       <c r="G167">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H167">
+        <v>0</v>
+      </c>
+      <c r="I167">
+        <v>0.92064500140678762</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>99564</v>
       </c>
@@ -4910,8 +5927,14 @@
       <c r="G168">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>0.92168647548360205</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>99565</v>
       </c>
@@ -4933,8 +5956,14 @@
       <c r="G169">
         <v>2.31</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>0.92479599579791216</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>99541</v>
       </c>
@@ -4956,8 +5985,14 @@
       <c r="G170">
         <v>2.87</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>0.92941892571429274</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>99576</v>
       </c>
@@ -4979,8 +6014,14 @@
       <c r="G171">
         <v>2.56</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H171">
+        <v>0</v>
+      </c>
+      <c r="I171">
+        <v>0.92941892571429274</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>99566</v>
       </c>
@@ -5002,8 +6043,14 @@
       <c r="G172">
         <v>4.43</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>0.92992956008458783</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>99570</v>
       </c>
@@ -5025,8 +6072,14 @@
       <c r="G173">
         <v>2.67</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>0.93145787068900499</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>99575</v>
       </c>
@@ -5048,8 +6101,14 @@
       <c r="G174">
         <v>2.63</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>0.93449845124356767</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>99553</v>
       </c>
@@ -5071,8 +6130,14 @@
       <c r="G175">
         <v>4.8099999999999996</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H175">
+        <v>0</v>
+      </c>
+      <c r="I175">
+        <v>0.94001815500766328</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>99563</v>
       </c>
@@ -5094,8 +6159,14 @@
       <c r="G176">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H176">
+        <v>0</v>
+      </c>
+      <c r="I176">
+        <v>0.94250410616808067</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>99568</v>
       </c>
@@ -5117,8 +6188,14 @@
       <c r="G177">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>0.95999483832841614</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>74658</v>
       </c>
@@ -5140,8 +6217,14 @@
       <c r="G178">
         <v>1.85</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H178">
+        <v>0</v>
+      </c>
+      <c r="I178">
+        <v>0.96378782734555524</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>99535</v>
       </c>
@@ -5163,8 +6246,14 @@
       <c r="G179">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179">
+        <v>0.98407703390283086</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>99528</v>
       </c>
@@ -5186,8 +6275,14 @@
       <c r="G180">
         <v>2.42</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H180">
+        <v>0</v>
+      </c>
+      <c r="I180">
+        <v>0.99078269180313783</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>99545</v>
       </c>
@@ -5209,8 +6304,14 @@
       <c r="G181">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181">
+        <v>0.99255351783213563</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>99534</v>
       </c>
@@ -5232,8 +6333,14 @@
       <c r="G182">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182">
+        <v>1.0102999566398119</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>74673</v>
       </c>
@@ -5255,8 +6362,14 @@
       <c r="G183">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>1.0232524596337116</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>99530</v>
       </c>
@@ -5278,8 +6391,14 @@
       <c r="G184">
         <v>2.97</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>1.0310042813635367</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>99539</v>
       </c>
@@ -5301,8 +6420,14 @@
       <c r="G185">
         <v>5.29</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H185">
+        <v>0</v>
+      </c>
+      <c r="I185">
+        <v>1.0334237554869496</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>74672</v>
       </c>
@@ -5324,8 +6449,14 @@
       <c r="G186">
         <v>4.79</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186">
+        <v>1.0472748673841794</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>99542</v>
       </c>
@@ -5347,8 +6478,14 @@
       <c r="G187">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187">
+        <v>1.0530784434834197</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>99529</v>
       </c>
@@ -5370,8 +6507,14 @@
       <c r="G188">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>1.055378331375</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>99544</v>
       </c>
@@ -5393,8 +6536,14 @@
       <c r="G189">
         <v>3.88</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H189">
+        <v>0</v>
+      </c>
+      <c r="I189">
+        <v>1.0845762779343311</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>74661</v>
       </c>
@@ -5416,8 +6565,14 @@
       <c r="G190">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H190">
+        <v>0</v>
+      </c>
+      <c r="I190">
+        <v>1.0962145853464051</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>24934</v>
       </c>
@@ -5439,8 +6594,14 @@
       <c r="G191">
         <v>4.1100000000000003</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H191">
+        <v>0</v>
+      </c>
+      <c r="I191">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>74649</v>
       </c>
@@ -5462,8 +6623,14 @@
       <c r="G192">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H192">
+        <v>0</v>
+      </c>
+      <c r="I192">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>74654</v>
       </c>
@@ -5485,8 +6652,14 @@
       <c r="G193">
         <v>3.38</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>74657</v>
       </c>
@@ -5508,8 +6681,14 @@
       <c r="G194">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>74680</v>
       </c>
@@ -5531,8 +6710,14 @@
       <c r="G195">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>99531</v>
       </c>
@@ -5554,8 +6739,14 @@
       <c r="G196">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H196">
+        <v>0</v>
+      </c>
+      <c r="I196">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>99532</v>
       </c>
@@ -5577,8 +6768,14 @@
       <c r="G197">
         <v>2.78</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="I197">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>99537</v>
       </c>
@@ -5600,8 +6797,14 @@
       <c r="G198">
         <v>2.4700000000000002</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>99538</v>
       </c>
@@ -5623,8 +6826,14 @@
       <c r="G199">
         <v>1.17</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H199">
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>99546</v>
       </c>
@@ -5646,8 +6855,14 @@
       <c r="G200">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H200">
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <v>1.3979400086720377</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>99547</v>
       </c>
@@ -5668,6 +6883,12 @@
       </c>
       <c r="G201">
         <v>3.02</v>
+      </c>
+      <c r="H201">
+        <v>0</v>
+      </c>
+      <c r="I201">
+        <v>1.3979400086720377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>